<commit_message>
Add med case results to spreadsheet
</commit_message>
<xml_diff>
--- a/use_cases/LWRS/LWRS_results.xlsx
+++ b/use_cases/LWRS/LWRS_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWRS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58ECC451-88E0-A240-A712-8A3DD34236A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED4AF1C-4FDE-0848-9B11-0A761C877BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{9EE474E5-2592-4044-A45A-603D647FE853}"/>
   </bookViews>
@@ -437,7 +437,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -479,9 +479,15 @@
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="e">
+      <c r="B3">
+        <v>6351431704.04</v>
+      </c>
+      <c r="C3">
+        <v>6645541.1728499997</v>
+      </c>
+      <c r="D3" s="2">
         <f t="shared" ref="D3:D9" si="0">C3/B3</f>
-        <v>#DIV/0!</v>
+        <v>1.046306011386838E-3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Set up delta NPV calculations and std deviation propagation
</commit_message>
<xml_diff>
--- a/use_cases/LWRS/LWRS_results.xlsx
+++ b/use_cases/LWRS/LWRS_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWRS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED4AF1C-4FDE-0848-9B11-0A761C877BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5187F315-53A4-C14F-B640-1FACEFD23AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{9EE474E5-2592-4044-A45A-603D647FE853}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Case</t>
   </si>
@@ -72,6 +72,18 @@
   </si>
   <si>
     <t>Std NPV (%)</t>
+  </si>
+  <si>
+    <t>Delta NPV</t>
+  </si>
+  <si>
+    <t>Std Delta NPV (upper bound)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Std Delta NPV (%)</t>
   </si>
 </sst>
 </file>
@@ -434,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B72939-7718-F04D-9ED0-21E4DB6080A0}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -446,7 +458,7 @@
     <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,8 +471,17 @@
       <c r="D1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -474,8 +495,15 @@
         <f>C2/B2</f>
         <v>2.5859333745341571E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <f>B2-$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -489,8 +517,20 @@
         <f t="shared" ref="D3:D9" si="0">C3/B3</f>
         <v>1.046306011386838E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <f t="shared" ref="E3:E9" si="1">B3-$B$2</f>
+        <v>2442827484.25</v>
+      </c>
+      <c r="F3">
+        <f>SQRT(POWER($C$2,2)+POWER(C3,2))</f>
+        <v>12096385.911071934</v>
+      </c>
+      <c r="G3" s="2">
+        <f>F3/E3</f>
+        <v>4.9517970421827729E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -504,8 +544,20 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>1470778551.9700003</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F9" si="2">SQRT(POWER($C$2,2)+POWER(C4,2))</f>
+        <v>10107390.0998</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G9" si="3">F4/E4</f>
+        <v>6.8721359080616794E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -519,8 +571,20 @@
         <f t="shared" si="0"/>
         <v>2.8511953924864171E-16</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>2797913013.75</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>10107390.0998</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="3"/>
+        <v>3.6124747446144583E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -534,8 +598,20 @@
         <f t="shared" si="0"/>
         <v>1.9277087156959612E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>-327567182.02999973</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>12239830.632366681</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="3"/>
+        <v>-3.736586356580042E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -543,8 +619,20 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>-3908604219.79</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>10107390.0998</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="3"/>
+        <v>-2.5859333745341571E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -552,14 +640,38 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>-3908604219.79</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>10107390.0998</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="3"/>
+        <v>-2.5859333745341571E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>-3908604219.79</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>10107390.0998</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="3"/>
+        <v>-2.5859333745341571E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set up table for tornado diagram
</commit_message>
<xml_diff>
--- a/use_cases/LWRS/LWRS_results.xlsx
+++ b/use_cases/LWRS/LWRS_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWRS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5187F315-53A4-C14F-B640-1FACEFD23AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30686FB9-FE83-F74D-AB96-FC724513BC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{9EE474E5-2592-4044-A45A-603D647FE853}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Case</t>
   </si>
@@ -84,6 +84,30 @@
   </si>
   <si>
     <t>Std Delta NPV (%)</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Electricity price</t>
+  </si>
+  <si>
+    <t>Synfuel price</t>
+  </si>
+  <si>
+    <t>Synfuel plant capacity</t>
+  </si>
+  <si>
+    <t>Std low</t>
+  </si>
+  <si>
+    <t>Std high</t>
   </si>
 </sst>
 </file>
@@ -446,15 +470,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B72939-7718-F04D-9ED0-21E4DB6080A0}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -674,6 +699,62 @@
         <v>-2.5859333745341571E-3</v>
       </c>
     </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <f>E4-E3</f>
+        <v>-972048932.27999973</v>
+      </c>
+      <c r="C12">
+        <f>E5-E3</f>
+        <v>355085529.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <f>E6-E3</f>
+        <v>-2770394666.2799997</v>
+      </c>
+      <c r="C13">
+        <f>E7-E3</f>
+        <v>-6351431704.04</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <f>E8-E3</f>
+        <v>-6351431704.04</v>
+      </c>
+      <c r="C14">
+        <f>-E9-E3</f>
+        <v>1465776735.54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add results for plant_cap_high and plant_cap_low
</commit_message>
<xml_diff>
--- a/use_cases/LWRS/LWRS_results.xlsx
+++ b/use_cases/LWRS/LWRS_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWRS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30686FB9-FE83-F74D-AB96-FC724513BC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E268160-7A4D-D64B-AA4D-916D6C06E787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{9EE474E5-2592-4044-A45A-603D647FE853}"/>
   </bookViews>
@@ -473,7 +473,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -661,34 +661,46 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="2" t="e">
+      <c r="B8">
+        <v>4238322741.1799998</v>
+      </c>
+      <c r="C8">
+        <v>9929293.0508699995</v>
+      </c>
+      <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>2.3427411401203404E-3</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>-3908604219.79</v>
+        <v>329718521.38999987</v>
       </c>
       <c r="F8">
         <f t="shared" si="2"/>
-        <v>10107390.0998</v>
+        <v>14168634.200923895</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="3"/>
-        <v>-2.5859333745341571E-3</v>
+        <v>4.2971908709261909E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="2" t="e">
+      <c r="B9">
+        <v>10696284773.200001</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1.9121349606199998E-6</v>
+      </c>
+      <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.7876627269787503E-16</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>-3908604219.79</v>
+        <v>6787680553.4100008</v>
       </c>
       <c r="F9">
         <f t="shared" si="2"/>
@@ -696,7 +708,7 @@
       </c>
       <c r="G9" s="2">
         <f t="shared" si="3"/>
-        <v>-2.5859333745341571E-3</v>
+        <v>1.4890786359594134E-3</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -748,11 +760,11 @@
       </c>
       <c r="B14">
         <f>E8-E3</f>
-        <v>-6351431704.04</v>
+        <v>-2113108962.8600001</v>
       </c>
       <c r="C14">
         <f>-E9-E3</f>
-        <v>1465776735.54</v>
+        <v>-9230508037.6599998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new elec high result to tornado chart plot
</commit_message>
<xml_diff>
--- a/use_cases/LWRS/LWRS_results.xlsx
+++ b/use_cases/LWRS/LWRS_results.xlsx
@@ -8,20 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWRS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA76DCE-E078-CE46-9C08-A7B93CC8B51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB9EF1B-6F6C-1242-8B92-9E51CB545AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{9EE474E5-2592-4044-A45A-603D647FE853}"/>
+    <workbookView xWindow="-37820" yWindow="1100" windowWidth="35840" windowHeight="19400" xr2:uid="{9EE474E5-2592-4044-A45A-603D647FE853}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$A$12:$A$14</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$B$11</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$B$12:$B$14</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">Sheet1!$C$11</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">Sheet1!$C$12:$C$14</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -362,7 +355,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>355085529.5</c:v>
+                  <c:v>1135971446.8199997</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2768833868.2699995</c:v>
@@ -405,7 +398,7 @@
         <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -504,6 +497,38 @@
         <c:crossBetween val="between"/>
         <c:majorUnit val="1000000000"/>
         <c:minorUnit val="500000000"/>
+        <c:dispUnits>
+          <c:builtInUnit val="billions"/>
+          <c:dispUnitsLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1101,12 +1126,12 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>719667</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>20108</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>56444</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>635001</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
@@ -1435,15 +1460,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B72939-7718-F04D-9ED0-21E4DB6080A0}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -1550,18 +1578,18 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>6706517233.54</v>
+        <v>7487403150.8599997</v>
       </c>
       <c r="C5" s="1">
         <v>1.91215910359E-6</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>2.8511953924864171E-16</v>
+        <v>2.5538348410828799E-16</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>2797913013.75</v>
+        <v>3578798931.0699997</v>
       </c>
       <c r="F5">
         <f t="shared" si="3"/>
@@ -1569,7 +1597,7 @@
       </c>
       <c r="G5" s="2">
         <f t="shared" si="2"/>
-        <v>3.6124747446144583E-3</v>
+        <v>2.8242408401463514E-3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1707,7 +1735,7 @@
       </c>
       <c r="C12">
         <f>E5-E3</f>
-        <v>355085529.5</v>
+        <v>1135971446.8199997</v>
       </c>
       <c r="D12">
         <f>SQRT(POWER($F$3,2)+POWER(F4,2))</f>

</xml_diff>

<commit_message>
Write input for hydrogen PTC, fix mistake in co2 cost function
</commit_message>
<xml_diff>
--- a/use_cases/LWRS/LWRS_results.xlsx
+++ b/use_cases/LWRS/LWRS_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWRS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB9EF1B-6F6C-1242-8B92-9E51CB545AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD33AD98-9AEE-C948-B29F-678419ECC8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37820" yWindow="1100" windowWidth="35840" windowHeight="19400" xr2:uid="{9EE474E5-2592-4044-A45A-603D647FE853}"/>
+    <workbookView xWindow="0" yWindow="1380" windowWidth="35840" windowHeight="19400" xr2:uid="{9EE474E5-2592-4044-A45A-603D647FE853}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Case</t>
   </si>
@@ -63,12 +63,6 @@
   </si>
   <si>
     <t>plant_cap_high</t>
-  </si>
-  <si>
-    <t>med (Ref for SA)</t>
-  </si>
-  <si>
-    <t>baseline_elec (REF REF)</t>
   </si>
   <si>
     <t>Std NPV (%)</t>
@@ -108,6 +102,18 @@
   </si>
   <si>
     <t>Std high</t>
+  </si>
+  <si>
+    <t>Baseline electricity</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Ref Ref</t>
+  </si>
+  <si>
+    <t>Ref for SA</t>
   </si>
 </sst>
 </file>
@@ -575,7 +581,393 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean NPV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Median</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6351431704.04</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B0FC-5949-B64D-88785D628AD9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="300"/>
+        <c:axId val="776062752"/>
+        <c:axId val="528268015"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="776062752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="528268015"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="528268015"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Δ NPV</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="776062752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="billions"/>
+          <c:dispUnitsLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1120,6 +1512,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1153,6 +2048,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>450851</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>635001</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>196272</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36302404-832A-171E-E2E4-DAB69B892A07}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1458,10 +2389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B72939-7718-F04D-9ED0-21E4DB6080A0}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E1" activeCellId="2" sqref="A3 E3 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1474,7 +2405,7 @@
     <col min="7" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1485,21 +2416,21 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>3908604219.79</v>
@@ -1516,12 +2447,15 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>6351431704.04</v>
@@ -1545,8 +2479,11 @@
         <f t="shared" ref="G3:G5" si="2">ABS(F3/E3)</f>
         <v>4.9517970421827729E-3</v>
       </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1573,7 +2510,7 @@
         <v>6.8721359080616794E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1600,7 +2537,7 @@
         <v>2.8242408401463514E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1627,7 +2564,7 @@
         <v>3.736586356580042E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1654,7 +2591,7 @@
         <v>2.2569147575074375E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1681,7 +2618,7 @@
         <v>4.2971908709261909E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1708,26 +2645,26 @@
         <v>1.4890786359594134E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>19</v>
       </c>
       <c r="B12">
         <f>E4-E3</f>
@@ -1746,9 +2683,9 @@
         <v>15763308.242215991</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <f>E6-E3</f>
@@ -1767,9 +2704,9 @@
         <v>16872275.338846456</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <f>E8-E3</f>

</xml_diff>

<commit_message>
Changing results file name
</commit_message>
<xml_diff>
--- a/use_cases/LWRS/LWRS_results.xlsx
+++ b/use_cases/LWRS/LWRS_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWRS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD33AD98-9AEE-C948-B29F-678419ECC8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4FD343-7083-8A46-9A21-671A218406E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1380" windowWidth="35840" windowHeight="19400" xr2:uid="{9EE474E5-2592-4044-A45A-603D647FE853}"/>
+    <workbookView xWindow="0" yWindow="920" windowWidth="35840" windowHeight="19400" xr2:uid="{9EE474E5-2592-4044-A45A-603D647FE853}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Case</t>
   </si>
@@ -115,12 +115,38 @@
   <si>
     <t>Ref for SA</t>
   </si>
+  <si>
+    <r>
+      <t>Median H</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> PTC</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -134,6 +160,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -153,16 +184,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -200,10 +233,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12653827436937254"/>
-          <c:y val="5.3967701234427588E-2"/>
-          <c:w val="0.83992402232901031"/>
-          <c:h val="0.87511548589017918"/>
+          <c:x val="0.16278172912733452"/>
+          <c:y val="6.8213035842477718E-2"/>
+          <c:w val="0.77525391993319726"/>
+          <c:h val="0.82973512156031126"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -215,7 +248,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$11</c:f>
+              <c:f>Sheet1!$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -226,27 +259,63 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent6"/>
+              <a:schemeClr val="accent6">
+                <a:alpha val="66000"/>
+              </a:schemeClr>
             </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
-            <c:errValType val="fixedVal"/>
+            <c:errValType val="cust"/>
             <c:noEndCap val="0"/>
-            <c:val val="1000000000"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$E$13:$E$15</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>15828445.080616167</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>17258366.63144559</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>15828445.080616167</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$D$13:$D$15</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>15828445.080616167</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>17190871.780215744</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>18919850.81651184</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
             <c:spPr>
               <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
@@ -255,7 +324,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$12:$A$14</c:f>
+              <c:f>Sheet1!$A$13:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -272,18 +341,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$B$14</c:f>
+              <c:f>Sheet1!$B$13:$B$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>-972048932.27999973</c:v>
+                  <c:v>-1063205222.8900003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2770394666.2799997</c:v>
+                  <c:v>-2061486996.0799999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2113108962.8600001</c:v>
+                  <c:v>-790038144.14000034</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -299,7 +368,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$11</c:f>
+              <c:f>Sheet1!$C$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -310,27 +379,63 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="accent2">
+                <a:alpha val="72000"/>
+              </a:schemeClr>
             </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
-            <c:errValType val="fixedVal"/>
+            <c:errValType val="cust"/>
             <c:noEndCap val="0"/>
-            <c:val val="1000000000"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$E$13:$E$15</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>15828445.080616167</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>17258366.63144559</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>15828445.080616167</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$D$13:$D$15</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>15828445.080616167</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>17190871.780215744</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>18919850.81651184</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
             <c:spPr>
               <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
@@ -339,7 +444,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$12:$A$14</c:f>
+              <c:f>Sheet1!$A$13:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -356,18 +461,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$12:$C$14</c:f>
+              <c:f>Sheet1!$C$13:$C$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1135971446.8199997</c:v>
+                  <c:v>1152047620.7200003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2768833868.2699995</c:v>
+                  <c:v>2055019080.4700003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4344853069.1600008</c:v>
+                  <c:v>5770030407.7600002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -420,7 +525,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -447,7 +552,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6000000000"/>
-          <c:min val="-4000000000"/>
+          <c:min val="-3000000000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -465,7 +570,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
@@ -483,7 +588,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -502,7 +607,7 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1000000000"/>
-        <c:minorUnit val="500000000"/>
+        <c:minorUnit val="250000000"/>
         <c:dispUnits>
           <c:builtInUnit val="billions"/>
           <c:dispUnitsLbl>
@@ -599,7 +704,7 @@
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="col"/>
+        <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -618,33 +723,88 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent1">
+                <a:alpha val="64000"/>
+              </a:schemeClr>
             </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="25400">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$F$3:$F$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>12181146.868852172</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>10992051.970760122</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$F$3:$F$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>12181146.868852172</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>10992051.970760122</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="28575" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3</c:f>
+              <c:f>Sheet1!$A$3:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>Median</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Median H2 PTC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3</c:f>
+              <c:f>Sheet1!$E$3:$E$4</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>6351431704.04</c:v>
+                  <c:v>639575960.55000019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2269920874.9700003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -673,7 +833,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -722,9 +882,10 @@
         <c:axId val="528268015"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -756,7 +917,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -788,7 +949,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -853,7 +1014,403 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean NPV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="64000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="25400">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$F$3:$F$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>12181146.868852172</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>10992051.970760122</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$F$3:$F$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>12181146.868852172</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>10992051.970760122</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="28575" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Median</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>639575960.55000019</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F3DA-1B4E-AA13-C7DD1AF36678}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="300"/>
+        <c:axId val="776062752"/>
+        <c:axId val="528268015"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="776062752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="528268015"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="528268015"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Δ NPV</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="776062752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+          <c:dispUnitsLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -1007,6 +1564,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -1513,6 +2110,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2020,15 +3120,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>719667</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>56444</xdr:rowOff>
+      <xdr:colOff>65617</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>3527</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2055,16 +3155,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>450851</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>184149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>635001</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>196272</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>260350</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2084,6 +3184,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>196850</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{029D3ADC-DB77-0944-9DCB-DF5DD35CE67F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2389,18 +3527,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B72939-7718-F04D-9ED0-21E4DB6080A0}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E1" activeCellId="2" sqref="A3 E3 E1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2432,21 +3571,21 @@
       <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>3908604219.79</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>10107390.0998</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <f>C2/B2</f>
         <v>2.5859333745341571E-3</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <f>B2-$B$2</f>
         <v>0</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
@@ -2457,27 +3596,27 @@
       <c r="A3" t="s">
         <v>23</v>
       </c>
-      <c r="B3">
-        <v>6351431704.04</v>
-      </c>
-      <c r="C3">
-        <v>6645541.1728499997</v>
-      </c>
-      <c r="D3" s="2">
-        <f t="shared" ref="D3:D9" si="0">C3/B3</f>
-        <v>1.046306011386838E-3</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E9" si="1">B3-$B$2</f>
-        <v>2442827484.25</v>
-      </c>
-      <c r="F3">
+      <c r="B3" s="2">
+        <v>4548180180.3400002</v>
+      </c>
+      <c r="C3" s="2">
+        <v>6798603.1220399998</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D10" si="0">C3/B3</f>
+        <v>1.4947963476530011E-3</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E10" si="1">B3-$B$2</f>
+        <v>639575960.55000019</v>
+      </c>
+      <c r="F3" s="2">
         <f>SQRT(POWER($C$2,2)+POWER(C3,2))</f>
-        <v>12096385.911071934</v>
-      </c>
-      <c r="G3" s="2">
-        <f t="shared" ref="G3:G5" si="2">ABS(F3/E3)</f>
-        <v>4.9517970421827729E-3</v>
+        <v>12181146.868852172</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G10" si="2">ABS(F3/E3)</f>
+        <v>1.9045660906918789E-2</v>
       </c>
       <c r="H3" t="s">
         <v>25</v>
@@ -2485,244 +3624,274 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>5379382771.7600002</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
+        <v>26</v>
+      </c>
+      <c r="B4" s="2">
+        <v>6178525094.7600002</v>
+      </c>
+      <c r="C4" s="2">
+        <v>4320401.8213999998</v>
+      </c>
+      <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="1"/>
-        <v>1470778551.9700003</v>
-      </c>
-      <c r="F4">
-        <f t="shared" ref="F4:F9" si="3">SQRT(POWER($C$2,2)+POWER(C4,2))</f>
-        <v>10107390.0998</v>
-      </c>
-      <c r="G4" s="2">
+        <v>6.9926102996071464E-4</v>
+      </c>
+      <c r="E4" s="2">
+        <f>B4-$B$2</f>
+        <v>2269920874.9700003</v>
+      </c>
+      <c r="F4" s="2">
+        <f>SQRT(POWER($C$2,2)+POWER(C4,2))</f>
+        <v>10992051.970760122</v>
+      </c>
+      <c r="G4" s="1">
         <f t="shared" si="2"/>
-        <v>6.8721359080616794E-3</v>
+        <v>4.8424824371490023E-3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>7487403150.8599997</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1.91215910359E-6</v>
-      </c>
-      <c r="D5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3484974957.4499998</v>
+      </c>
+      <c r="C5" s="2">
+        <v>5.0263049764099996E-7</v>
+      </c>
+      <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>2.5538348410828799E-16</v>
-      </c>
-      <c r="E5">
+        <v>1.4422786498551515E-16</v>
+      </c>
+      <c r="E5" s="2">
         <f t="shared" si="1"/>
-        <v>3578798931.0699997</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="3"/>
+        <v>-423629262.34000015</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" ref="F5:F10" si="3">SQRT(POWER($C$2,2)+POWER(C5,2))</f>
         <v>10107390.0998</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <f t="shared" si="2"/>
-        <v>2.8242408401463514E-3</v>
+        <v>2.3859046100757602E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>3581037037.7600002</v>
-      </c>
-      <c r="C6">
-        <v>6903196.3089199997</v>
-      </c>
-      <c r="D6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5700227801.0600004</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.96215910359E-6</v>
+      </c>
+      <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>1.9277087156959612E-3</v>
-      </c>
-      <c r="E6">
+        <v>3.4422468225307095E-16</v>
+      </c>
+      <c r="E6" s="2">
         <f t="shared" si="1"/>
-        <v>-327567182.02999973</v>
-      </c>
-      <c r="F6">
+        <v>1791623581.2700005</v>
+      </c>
+      <c r="F6" s="2">
         <f t="shared" si="3"/>
-        <v>12239830.632366681</v>
-      </c>
-      <c r="G6" s="2">
-        <f>ABS(F6/E6)</f>
-        <v>3.736586356580042E-2</v>
+        <v>10107390.0998</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="2"/>
+        <v>5.6414696733536685E-3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>9120265572.3099995</v>
-      </c>
-      <c r="C7">
-        <v>6015961.1344100004</v>
-      </c>
-      <c r="D7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2486693184.2600002</v>
+      </c>
+      <c r="C7" s="2">
+        <v>6707190.08928</v>
+      </c>
+      <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>6.5962565308131326E-4</v>
-      </c>
-      <c r="E7">
+        <v>2.6972326669548303E-3</v>
+      </c>
+      <c r="E7" s="2">
         <f t="shared" si="1"/>
-        <v>5211661352.5199995</v>
-      </c>
-      <c r="F7">
+        <v>-1421911035.5299997</v>
+      </c>
+      <c r="F7" s="2">
         <f t="shared" si="3"/>
-        <v>11762275.417633558</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" ref="G7:G9" si="4">ABS(F7/E7)</f>
-        <v>2.2569147575074375E-3</v>
+        <v>12130364.113383856</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="2"/>
+        <v>8.5310288831554164E-3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>4238322741.1799998</v>
-      </c>
-      <c r="C8">
-        <v>9929293.0508699995</v>
-      </c>
-      <c r="D8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>6603199260.8100004</v>
+      </c>
+      <c r="C8" s="2">
+        <v>6878338.8339999998</v>
+      </c>
+      <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>2.3427411401203404E-3</v>
-      </c>
-      <c r="E8">
+        <v>1.0416676163057736E-3</v>
+      </c>
+      <c r="E8" s="2">
         <f t="shared" si="1"/>
-        <v>329718521.38999987</v>
-      </c>
-      <c r="F8">
+        <v>2694595041.0200005</v>
+      </c>
+      <c r="F8" s="2">
         <f t="shared" si="3"/>
-        <v>14168634.200923895</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" si="4"/>
-        <v>4.2971908709261909E-2</v>
+        <v>12225828.386855736</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="2"/>
+        <v>4.537167255465528E-3</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3758142036.1999998</v>
+      </c>
+      <c r="C9" s="2">
+        <v>10364414.1778</v>
+      </c>
+      <c r="D9" s="1">
+        <f>C9/B9</f>
+        <v>2.7578558973997301E-3</v>
+      </c>
+      <c r="E9" s="2">
+        <f>B9-$B$2</f>
+        <v>-150462183.59000015</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="3"/>
+        <v>14476892.480035786</v>
+      </c>
+      <c r="G9" s="1">
+        <f>ABS(F9/E9)</f>
+        <v>9.6216153020112966E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>10696284773.200001</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1.9121349606199998E-6</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="B10" s="2">
+        <v>10318210588.1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>3.8799104897699997E-6</v>
+      </c>
+      <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>1.7876627269787503E-16</v>
-      </c>
-      <c r="E9">
+        <v>3.7602551882830375E-16</v>
+      </c>
+      <c r="E10" s="2">
         <f t="shared" si="1"/>
-        <v>6787680553.4100008</v>
-      </c>
-      <c r="F9">
+        <v>6409606368.3100004</v>
+      </c>
+      <c r="F10" s="2">
         <f t="shared" si="3"/>
         <v>10107390.0998</v>
       </c>
-      <c r="G9" s="2">
-        <f t="shared" si="4"/>
-        <v>1.4890786359594134E-3</v>
+      <c r="G10" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5769127648419044E-3</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" t="s">
-        <v>21</v>
-      </c>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12">
-        <f>E4-E3</f>
-        <v>-972048932.27999973</v>
-      </c>
-      <c r="C12">
-        <f>E5-E3</f>
-        <v>1135971446.8199997</v>
-      </c>
-      <c r="D12">
-        <f>SQRT(POWER($F$3,2)+POWER(F4,2))</f>
-        <v>15763308.242215991</v>
-      </c>
-      <c r="E12">
-        <f>SQRT(POWER($F$3,2)+POWER(F5,2))</f>
-        <v>15763308.242215991</v>
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13">
+        <v>17</v>
+      </c>
+      <c r="B13" s="2">
+        <f>E5-E3</f>
+        <v>-1063205222.8900003</v>
+      </c>
+      <c r="C13" s="2">
         <f>E6-E3</f>
-        <v>-2770394666.2799997</v>
-      </c>
-      <c r="C13">
-        <f>E7-E3</f>
-        <v>2768833868.2699995</v>
-      </c>
-      <c r="D13">
+        <v>1152047620.7200003</v>
+      </c>
+      <c r="D13" s="2">
+        <f>SQRT(POWER($F$3,2)+POWER(F5,2))</f>
+        <v>15828445.080616167</v>
+      </c>
+      <c r="E13" s="2">
         <f>SQRT(POWER($F$3,2)+POWER(F6,2))</f>
-        <v>17208602.67478453</v>
-      </c>
-      <c r="E13">
-        <f>SQRT(POWER($F$3,2)+POWER(F7,2))</f>
-        <v>16872275.338846456</v>
+        <v>15828445.080616167</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2">
+        <f>E7-E3</f>
+        <v>-2061486996.0799999</v>
+      </c>
+      <c r="C14" s="2">
+        <f>E8-E3</f>
+        <v>2055019080.4700003</v>
+      </c>
+      <c r="D14" s="2">
+        <f>SQRT(POWER($F$3,2)+POWER(F7,2))</f>
+        <v>17190871.780215744</v>
+      </c>
+      <c r="E14" s="2">
+        <f>SQRT(POWER($F$3,2)+POWER(F8,2))</f>
+        <v>17258366.63144559</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="B14">
-        <f>E8-E3</f>
-        <v>-2113108962.8600001</v>
-      </c>
-      <c r="C14">
+      <c r="B15" s="2">
         <f>E9-E3</f>
-        <v>4344853069.1600008</v>
-      </c>
-      <c r="D14">
-        <f>SQRT(POWER($F$3,2)+POWER(F8,2))</f>
-        <v>18629888.545806438</v>
-      </c>
-      <c r="E14">
+        <v>-790038144.14000034</v>
+      </c>
+      <c r="C15" s="2">
+        <f>E10-E3</f>
+        <v>5770030407.7600002</v>
+      </c>
+      <c r="D15" s="2">
         <f>SQRT(POWER($F$3,2)+POWER(F9,2))</f>
-        <v>15763308.242215991</v>
+        <v>18919850.81651184</v>
+      </c>
+      <c r="E15" s="2">
+        <f>SQRT(POWER($F$3,2)+POWER(F10,2))</f>
+        <v>15828445.080616167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add well formatted tornado plot
</commit_message>
<xml_diff>
--- a/use_cases/LWRS/LWRS_results.xlsx
+++ b/use_cases/LWRS/LWRS_results.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWRS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4FD343-7083-8A46-9A21-671A218406E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BBC3045-773A-E14B-9716-8EAB89C3672F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="920" windowWidth="35840" windowHeight="19400" xr2:uid="{9EE474E5-2592-4044-A45A-603D647FE853}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" xr2:uid="{9EE474E5-2592-4044-A45A-603D647FE853}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Case</t>
   </si>
@@ -138,6 +137,27 @@
       <t xml:space="preserve"> PTC</t>
     </r>
   </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>https://mbounthavong.com/blog/2018/5/26/communicating-data-effectively-with-data-visualizations-tornado-diagram</t>
+  </si>
+  <si>
+    <t>Guide for building a tornado chart with an offset x-axis</t>
+  </si>
+  <si>
+    <t>Synfuel Products Price</t>
+  </si>
+  <si>
+    <t>Electricity Price</t>
+  </si>
+  <si>
+    <t>Synfuel Plant Capacity</t>
+  </si>
 </sst>
 </file>
 
@@ -189,10 +209,11 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -525,7 +546,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -588,7 +609,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1004,7 +1025,7 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
-          <c:builtInUnit val="billions"/>
+          <c:builtInUnit val="millions"/>
           <c:dispUnitsLbl>
             <c:spPr>
               <a:noFill/>
@@ -1102,7 +1123,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1113,23 +1134,15 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Mean NPV</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>low</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1">
-                <a:alpha val="64000"/>
+                <a:alpha val="70298"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:ln w="25400">
+            <a:ln w="15875">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -1137,45 +1150,110 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="&quot;$&quot;#,##0.0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$F$3:$F$4</c:f>
+                <c:f>Sheet1!$D$13:$D$15</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="2"/>
+                  <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>12181146.868852172</c:v>
+                    <c:v>15828445.080616167</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>10992051.970760122</c:v>
+                    <c:v>17190871.780215744</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>18919850.81651184</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$F$3:$F$4</c:f>
+                <c:f>Sheet1!$D$13:$D$15</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="2"/>
+                  <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>12181146.868852172</c:v>
+                    <c:v>15828445.080616167</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>10992051.970760122</c:v>
+                    <c:v>17190871.780215744</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>18919850.81651184</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:minus>
             <c:spPr>
               <a:noFill/>
-              <a:ln w="28575" cap="flat" cmpd="sng" algn="ctr">
+              <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="tx1"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
@@ -1184,30 +1262,213 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3</c:f>
+              <c:f>Sheet1!$Q$33:$Q$35</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Median</c:v>
+                  <c:v>Synfuel Plant Capacity</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Synfuel Products Price</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Electricity Price</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3</c:f>
+              <c:f>Sheet1!$R$33:$R$35</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>639575960.55000019</c:v>
+                  <c:v>-150462183.59000015</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1421911035.5299997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-423629262.34000015</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F3DA-1B4E-AA13-C7DD1AF36678}"/>
+              <c16:uniqueId val="{00000000-BE56-4BDC-BC15-F44061235E3D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>high</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:alpha val="69690"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="15875">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="&quot;$&quot;#,##0.0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$E$13:$E$15</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>15828445.080616167</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>17258366.63144559</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>15828445.080616167</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$E$13:$E$15</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>15828445.080616167</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>17258366.63144559</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>15828445.080616167</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$Q$33:$Q$35</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Synfuel Plant Capacity</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Synfuel Products Price</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Electricity Price</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$S$33:$S$35</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6409606368.3100004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2694595041.0200005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1791623581.2700005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BE56-4BDC-BC15-F44061235E3D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1219,29 +1480,27 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="300"/>
-        <c:axId val="776062752"/>
-        <c:axId val="528268015"/>
+        <c:gapWidth val="182"/>
+        <c:overlap val="100"/>
+        <c:axId val="678771839"/>
+        <c:axId val="678772671"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="776062752"/>
+        <c:axId val="678771839"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1252,7 +1511,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1267,21 +1526,20 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="528268015"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="678772671"/>
+        <c:crossesAt val="639575961"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="528268015"/>
+        <c:axId val="678772671"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1296,77 +1554,8 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>Δ NPV</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
+        <c:numFmt formatCode="&quot;$&quot;#,##0.0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1381,7 +1570,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1396,11 +1585,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="776062752"/>
+        <c:crossAx val="678771839"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="1000000000"/>
         <c:dispUnits>
-          <c:builtInUnit val="millions"/>
+          <c:builtInUnit val="billions"/>
           <c:dispUnitsLbl>
             <c:spPr>
               <a:noFill/>
@@ -1414,7 +1604,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -2613,7 +2803,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2817,22 +3007,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2937,8 +3128,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3070,19 +3261,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3125,10 +3317,10 @@
       <xdr:rowOff>3527</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>95251</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3155,16 +3347,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>184149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>260350</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3191,29 +3383,27 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>660400</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>136524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>196850</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>177799</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{029D3ADC-DB77-0944-9DCB-DF5DD35CE67F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3910B936-5B6E-9AA9-33CB-AC816AA102D1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3527,24 +3717,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B72939-7718-F04D-9ED0-21E4DB6080A0}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3567,7 +3760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -3592,7 +3785,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -3621,8 +3814,12 @@
       <c r="H3" t="s">
         <v>25</v>
       </c>
+      <c r="J3" s="3">
+        <f>E4-E3</f>
+        <v>1630344914.4200001</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -3649,7 +3846,7 @@
         <v>4.8424824371490023E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3676,7 +3873,7 @@
         <v>2.3859046100757602E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3703,7 +3900,7 @@
         <v>5.6414696733536685E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3730,7 +3927,7 @@
         <v>8.5310288831554164E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3757,7 +3954,7 @@
         <v>4.537167255465528E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3784,7 +3981,7 @@
         <v>9.6216153020112966E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3811,10 +4008,10 @@
         <v>1.5769127648419044E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -3831,7 +4028,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -3852,7 +4049,7 @@
         <v>15828445.080616167</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -3873,7 +4070,7 @@
         <v>17258366.63144559</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -3892,6 +4089,63 @@
       <c r="E15" s="2">
         <f>SQRT(POWER($F$3,2)+POWER(F10,2))</f>
         <v>15828445.080616167</v>
+      </c>
+    </row>
+    <row r="28" spans="17:19" x14ac:dyDescent="0.2">
+      <c r="Q28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="17:19" x14ac:dyDescent="0.2">
+      <c r="Q29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="17:19" x14ac:dyDescent="0.2">
+      <c r="R32" t="s">
+        <v>27</v>
+      </c>
+      <c r="S32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="17:19" x14ac:dyDescent="0.2">
+      <c r="Q33" t="s">
+        <v>33</v>
+      </c>
+      <c r="R33" s="3">
+        <f>E9</f>
+        <v>-150462183.59000015</v>
+      </c>
+      <c r="S33" s="3">
+        <f>E10</f>
+        <v>6409606368.3100004</v>
+      </c>
+    </row>
+    <row r="34" spans="17:19" x14ac:dyDescent="0.2">
+      <c r="Q34" t="s">
+        <v>31</v>
+      </c>
+      <c r="R34" s="3">
+        <f>E7</f>
+        <v>-1421911035.5299997</v>
+      </c>
+      <c r="S34" s="3">
+        <f>E8</f>
+        <v>2694595041.0200005</v>
+      </c>
+    </row>
+    <row r="35" spans="17:19" x14ac:dyDescent="0.2">
+      <c r="Q35" t="s">
+        <v>32</v>
+      </c>
+      <c r="R35" s="3">
+        <f>E5</f>
+        <v>-423629262.34000015</v>
+      </c>
+      <c r="S35" s="3">
+        <f>E6</f>
+        <v>1791623581.2700005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>